<commit_message>
Changes in the Organization DetailView.
</commit_message>
<xml_diff>
--- a/esms/tracker/ESMS_Tracker.xlsx
+++ b/esms/tracker/ESMS_Tracker.xlsx
@@ -13,9 +13,10 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Story!$AC$3:$AC$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Story!$A$1:$Q$45</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -459,7 +460,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="267">
   <si>
     <t>Column</t>
   </si>
@@ -1210,6 +1211,57 @@
   </si>
   <si>
     <t>Create a new opportunity for an organization.</t>
+  </si>
+  <si>
+    <t>PRODUCT_ID</t>
+  </si>
+  <si>
+    <t>STATUS_ID</t>
+  </si>
+  <si>
+    <t>DATETIME_RECEIVED</t>
+  </si>
+  <si>
+    <t>DATETIME_MANUFACTURED</t>
+  </si>
+  <si>
+    <t>EXPIRE_DATE</t>
+  </si>
+  <si>
+    <t>LOT_ID</t>
+  </si>
+  <si>
+    <t>UOM_ID</t>
+  </si>
+  <si>
+    <t>COMMENTS</t>
+  </si>
+  <si>
+    <t>QUANTITY_ON_HAND_TOTAL</t>
+  </si>
+  <si>
+    <t>AVAILABLE_TO_PROMISE_TOTAL</t>
+  </si>
+  <si>
+    <t>QUANTITY_ON_HAND</t>
+  </si>
+  <si>
+    <t>AVAILABLE_TO_PROMISE</t>
+  </si>
+  <si>
+    <t>SERIAL_NUMBER</t>
+  </si>
+  <si>
+    <t>ACTIVATION_VALID_THRU</t>
+  </si>
+  <si>
+    <t>UNIT_COST</t>
+  </si>
+  <si>
+    <t>INVENTORY_ITEM_TYPE</t>
+  </si>
+  <si>
+    <t>Inventory Item</t>
   </si>
 </sst>
 </file>
@@ -1315,313 +1367,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <font>
         <condense val="0"/>
@@ -1715,6 +1461,70 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2008,15 +1818,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D136"/>
+  <dimension ref="A1:D155"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="A159" sqref="A159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="27" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
@@ -2869,18 +2679,125 @@
         <v>77</v>
       </c>
     </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" s="2" customFormat="1">
+      <c r="A139" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AC45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2946,7 +2863,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="25.5">
+    <row r="2" spans="1:29" hidden="1">
       <c r="A2" s="1" t="s">
         <v>115</v>
       </c>
@@ -2972,7 +2889,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="38.25">
+    <row r="3" spans="1:29" hidden="1">
       <c r="A3" s="1" t="s">
         <v>121</v>
       </c>
@@ -2998,7 +2915,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="25.5">
+    <row r="4" spans="1:29" ht="25.5" hidden="1">
       <c r="A4" s="1" t="s">
         <v>126</v>
       </c>
@@ -3024,7 +2941,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="25.5">
+    <row r="5" spans="1:29" ht="25.5" hidden="1">
       <c r="A5" s="1" t="s">
         <v>129</v>
       </c>
@@ -3050,7 +2967,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="38.25">
+    <row r="6" spans="1:29" ht="25.5" hidden="1">
       <c r="A6" s="1" t="s">
         <v>130</v>
       </c>
@@ -3076,7 +2993,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="25.5">
+    <row r="7" spans="1:29" ht="25.5" hidden="1">
       <c r="A7" s="1" t="s">
         <v>134</v>
       </c>
@@ -3102,7 +3019,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="25.5">
+    <row r="8" spans="1:29" ht="25.5" hidden="1">
       <c r="A8" s="1" t="s">
         <v>137</v>
       </c>
@@ -3128,7 +3045,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="38.25">
+    <row r="9" spans="1:29" ht="25.5">
       <c r="A9" s="1" t="s">
         <v>140</v>
       </c>
@@ -3154,7 +3071,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="25.5">
+    <row r="10" spans="1:29" ht="25.5" hidden="1">
       <c r="A10" s="1" t="s">
         <v>143</v>
       </c>
@@ -3177,7 +3094,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="25.5">
+    <row r="11" spans="1:29" ht="25.5" hidden="1">
       <c r="A11" s="1" t="s">
         <v>146</v>
       </c>
@@ -3200,7 +3117,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:29" hidden="1">
       <c r="A12" s="1" t="s">
         <v>149</v>
       </c>
@@ -3223,7 +3140,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="38.25">
+    <row r="13" spans="1:29" ht="25.5">
       <c r="A13" s="1" t="s">
         <v>152</v>
       </c>
@@ -3246,7 +3163,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="25.5">
+    <row r="14" spans="1:29" ht="25.5" hidden="1">
       <c r="A14" s="1" t="s">
         <v>155</v>
       </c>
@@ -3292,7 +3209,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="25.5">
+    <row r="16" spans="1:29" ht="25.5" hidden="1">
       <c r="A16" s="1" t="s">
         <v>161</v>
       </c>
@@ -3306,7 +3223,7 @@
         <v>163</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>167</v>
+        <v>119</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>120</v>
@@ -3338,7 +3255,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" hidden="1">
       <c r="A18" s="1" t="s">
         <v>169</v>
       </c>
@@ -3352,7 +3269,7 @@
         <v>171</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>167</v>
+        <v>119</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>120</v>
@@ -3582,7 +3499,7 @@
         <v>199</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>167</v>
+        <v>119</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>124</v>
@@ -3706,7 +3623,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" hidden="1">
       <c r="A34" s="1" t="s">
         <v>218</v>
       </c>
@@ -3752,7 +3669,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="25.5">
+    <row r="36" spans="1:10" ht="25.5" hidden="1">
       <c r="A36" s="1" t="s">
         <v>224</v>
       </c>
@@ -3766,7 +3683,7 @@
         <v>225</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>167</v>
+        <v>119</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>120</v>
@@ -3775,7 +3692,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="25.5">
+    <row r="37" spans="1:10" ht="25.5" hidden="1">
       <c r="A37" s="1" t="s">
         <v>226</v>
       </c>
@@ -3789,7 +3706,7 @@
         <v>227</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>167</v>
+        <v>119</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>120</v>
@@ -3983,39 +3900,46 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Q45">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Design"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="F1:G1">
-    <cfRule type="cellIs" dxfId="29" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
       <formula>"Must"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1">
-    <cfRule type="cellIs" dxfId="28" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>"Could"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>"Should"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="26" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
       <formula>"Implement"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"Design"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
       <formula>"Must"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"Could"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"Should"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4104,33 +4028,33 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="P1">
-    <cfRule type="cellIs" dxfId="38" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1">
-    <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Issue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Raised"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>"Withdrawn"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated the Work Tracker sheet.
</commit_message>
<xml_diff>
--- a/esms/tracker/ESMS_Tracker.xlsx
+++ b/esms/tracker/ESMS_Tracker.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="120" windowWidth="19155" windowHeight="11760" activeTab="1"/>
@@ -459,7 +459,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="295">
   <si>
     <t>Column</t>
   </si>
@@ -1291,13 +1291,67 @@
   </si>
   <si>
     <t>Attach inventory parts for repair sales order</t>
+  </si>
+  <si>
+    <t>S052</t>
+  </si>
+  <si>
+    <t>Create new quote from Organization/Lead Detail View.</t>
+  </si>
+  <si>
+    <t>Create a quote from the DetailView of Organization/Lead under the Quotes tab.</t>
+  </si>
+  <si>
+    <t>S053</t>
+  </si>
+  <si>
+    <t>Add a site address</t>
+  </si>
+  <si>
+    <t>While creating the Lead/Organization, divide the address box into 2 parts (left and right) to record the site address and the billing address.</t>
+  </si>
+  <si>
+    <t>Before the Quote is converted into a Sales Order, capture the Negotiated Final Amount</t>
+  </si>
+  <si>
+    <t>S054</t>
+  </si>
+  <si>
+    <t>Add a new Contracter.</t>
+  </si>
+  <si>
+    <t>S055</t>
+  </si>
+  <si>
+    <t>View the Line Items assignments.</t>
+  </si>
+  <si>
+    <t>View the line items assignments to external contracters, if any, in the tab shown in the Quote DetailView.</t>
+  </si>
+  <si>
+    <t>S056</t>
+  </si>
+  <si>
+    <t>View the Order Status History</t>
+  </si>
+  <si>
+    <t>View the status changes for the Order.</t>
+  </si>
+  <si>
+    <t>S057</t>
+  </si>
+  <si>
+    <t>View the maintenance work orders in a different tab.</t>
+  </si>
+  <si>
+    <t>View the Maintenance Work Orders in a different tab other that order.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1403,7 +1457,139 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="29">
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -1566,6 +1752,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1644,6 +1835,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1678,6 +1870,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1853,14 +2046,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D167"/>
   <sheetViews>
     <sheetView topLeftCell="A151" workbookViewId="0">
       <selection activeCell="D170" sqref="D170"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.140625" style="1"/>
@@ -1868,12 +2061,12 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1">
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1884,47 +2077,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1938,12 +2131,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="2" customFormat="1">
+    <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -1954,7 +2147,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1965,7 +2158,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -1979,7 +2172,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1990,7 +2183,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -2004,12 +2197,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="2" customFormat="1">
+    <row r="21" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
@@ -2020,7 +2213,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -2031,7 +2224,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -2039,7 +2232,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
@@ -2050,7 +2243,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
@@ -2058,7 +2251,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -2066,7 +2259,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
@@ -2074,7 +2267,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
@@ -2088,7 +2281,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
@@ -2096,12 +2289,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="2" customFormat="1">
+    <row r="32" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>0</v>
       </c>
@@ -2112,7 +2305,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
@@ -2120,7 +2313,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -2128,7 +2321,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
@@ -2136,7 +2329,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
@@ -2144,7 +2337,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
@@ -2152,7 +2345,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
@@ -2160,7 +2353,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>42</v>
       </c>
@@ -2174,12 +2367,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:4" s="2" customFormat="1">
+    <row r="42" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>0</v>
       </c>
@@ -2190,12 +2383,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>22</v>
       </c>
@@ -2206,7 +2399,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>46</v>
       </c>
@@ -2214,12 +2407,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:4" s="2" customFormat="1">
+    <row r="48" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>0</v>
       </c>
@@ -2230,47 +2423,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>1</v>
       </c>
@@ -2278,17 +2471,17 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="61" spans="1:4" s="2" customFormat="1">
+    <row r="61" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>0</v>
       </c>
@@ -2299,12 +2492,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>32</v>
       </c>
@@ -2312,12 +2505,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>1</v>
       </c>
@@ -2325,27 +2518,27 @@
         <v>62</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>66</v>
       </c>
@@ -2356,32 +2549,32 @@
         <v>67</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="77" spans="1:4" s="2" customFormat="1">
+    <row r="77" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>0</v>
       </c>
@@ -2392,47 +2585,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="87" spans="1:4" s="2" customFormat="1">
+    <row r="87" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>0</v>
       </c>
@@ -2443,12 +2636,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>32</v>
       </c>
@@ -2456,12 +2649,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>1</v>
       </c>
@@ -2469,27 +2662,27 @@
         <v>62</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>66</v>
       </c>
@@ -2500,32 +2693,32 @@
         <v>67</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="103" spans="1:3" s="2" customFormat="1">
+    <row r="103" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>0</v>
       </c>
@@ -2536,47 +2729,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="113" spans="1:4" s="2" customFormat="1">
+    <row r="113" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>0</v>
       </c>
@@ -2587,12 +2780,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>32</v>
       </c>
@@ -2600,12 +2793,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>1</v>
       </c>
@@ -2613,27 +2806,27 @@
         <v>62</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>66</v>
       </c>
@@ -2644,32 +2837,32 @@
         <v>67</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="129" spans="1:3" s="2" customFormat="1">
+    <row r="129" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>0</v>
       </c>
@@ -2680,47 +2873,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="132" spans="1:3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="135" spans="1:3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="136" spans="1:3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="139" spans="1:3" s="2" customFormat="1">
+    <row r="139" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>0</v>
       </c>
@@ -2731,12 +2924,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="141" spans="1:3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>246</v>
       </c>
@@ -2744,7 +2937,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="142" spans="1:3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>247</v>
       </c>
@@ -2752,7 +2945,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="143" spans="1:3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>248</v>
       </c>
@@ -2760,67 +2953,67 @@
         <v>13</v>
       </c>
     </row>
-    <row r="144" spans="1:3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="150" spans="1:4">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="151" spans="1:4">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="152" spans="1:4">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="153" spans="1:4">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="154" spans="1:4">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="155" spans="1:4">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="157" spans="1:4">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" s="10" t="s">
         <v>263</v>
       </c>
@@ -2830,7 +3023,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="158" spans="1:4" s="2" customFormat="1">
+    <row r="158" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A158" s="10" t="s">
         <v>0</v>
       </c>
@@ -2842,7 +3035,7 @@
       </c>
       <c r="D158" s="10"/>
     </row>
-    <row r="159" spans="1:4">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" s="10" t="s">
         <v>264</v>
       </c>
@@ -2850,7 +3043,7 @@
       <c r="C159" s="10"/>
       <c r="D159" s="10"/>
     </row>
-    <row r="160" spans="1:4">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" s="10" t="s">
         <v>265</v>
       </c>
@@ -2860,7 +3053,7 @@
       </c>
       <c r="D160" s="10"/>
     </row>
-    <row r="161" spans="1:4">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" s="10" t="s">
         <v>266</v>
       </c>
@@ -2870,7 +3063,7 @@
       </c>
       <c r="D161" s="10"/>
     </row>
-    <row r="162" spans="1:4">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" s="10" t="s">
         <v>267</v>
       </c>
@@ -2880,7 +3073,7 @@
       </c>
       <c r="D162" s="10"/>
     </row>
-    <row r="163" spans="1:4">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" s="10" t="s">
         <v>268</v>
       </c>
@@ -2888,7 +3081,7 @@
       <c r="C163" s="10"/>
       <c r="D163" s="10"/>
     </row>
-    <row r="164" spans="1:4">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" s="10" t="s">
         <v>269</v>
       </c>
@@ -2896,7 +3089,7 @@
       <c r="C164" s="10"/>
       <c r="D164" s="10"/>
     </row>
-    <row r="165" spans="1:4">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" s="10" t="s">
         <v>270</v>
       </c>
@@ -2904,7 +3097,7 @@
       <c r="C165" s="10"/>
       <c r="D165" s="10"/>
     </row>
-    <row r="166" spans="1:4">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" s="10" t="s">
         <v>271</v>
       </c>
@@ -2912,7 +3105,7 @@
       <c r="C166" s="10"/>
       <c r="D166" s="10"/>
     </row>
-    <row r="167" spans="1:4">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" s="10" t="s">
         <v>272</v>
       </c>
@@ -2927,16 +3120,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AC45"/>
+  <dimension ref="A1:AC52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B53" sqref="A53:D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="26.42578125" style="9" bestFit="1" customWidth="1"/>
@@ -2946,7 +3139,7 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="7" customFormat="1" ht="54" customHeight="1">
+    <row r="1" spans="1:29" s="7" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>85</v>
       </c>
@@ -2999,7 +3192,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:29" hidden="1">
+    <row r="2" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>115</v>
       </c>
@@ -3025,7 +3218,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:29" hidden="1">
+    <row r="3" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>121</v>
       </c>
@@ -3051,7 +3244,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="25.5" hidden="1">
+    <row r="4" spans="1:29" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>126</v>
       </c>
@@ -3077,7 +3270,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="25.5" hidden="1">
+    <row r="5" spans="1:29" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>129</v>
       </c>
@@ -3103,7 +3296,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="25.5" hidden="1">
+    <row r="6" spans="1:29" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>130</v>
       </c>
@@ -3129,7 +3322,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="25.5" hidden="1">
+    <row r="7" spans="1:29" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>134</v>
       </c>
@@ -3155,7 +3348,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="25.5" hidden="1">
+    <row r="8" spans="1:29" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>137</v>
       </c>
@@ -3181,7 +3374,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="25.5">
+    <row r="9" spans="1:29" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>140</v>
       </c>
@@ -3207,7 +3400,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="25.5" hidden="1">
+    <row r="10" spans="1:29" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>143</v>
       </c>
@@ -3230,7 +3423,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="25.5" hidden="1">
+    <row r="11" spans="1:29" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>146</v>
       </c>
@@ -3253,7 +3446,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="12" spans="1:29" hidden="1">
+    <row r="12" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>149</v>
       </c>
@@ -3276,7 +3469,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="25.5">
+    <row r="13" spans="1:29" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>152</v>
       </c>
@@ -3290,7 +3483,7 @@
         <v>154</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>167</v>
+        <v>119</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>120</v>
@@ -3299,7 +3492,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="25.5" hidden="1">
+    <row r="14" spans="1:29" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>155</v>
       </c>
@@ -3322,7 +3515,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="15" spans="1:29" ht="25.5">
+    <row r="15" spans="1:29" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>158</v>
       </c>
@@ -3345,7 +3538,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="25.5" hidden="1">
+    <row r="16" spans="1:29" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>161</v>
       </c>
@@ -3368,7 +3561,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="25.5">
+    <row r="17" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>164</v>
       </c>
@@ -3391,7 +3584,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>169</v>
       </c>
@@ -3414,7 +3607,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="25.5">
+    <row r="19" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>172</v>
       </c>
@@ -3437,7 +3630,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="25.5">
+    <row r="20" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>175</v>
       </c>
@@ -3460,7 +3653,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>177</v>
       </c>
@@ -3474,7 +3667,7 @@
         <v>179</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>167</v>
+        <v>119</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>120</v>
@@ -3483,7 +3676,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>180</v>
       </c>
@@ -3497,7 +3690,7 @@
         <v>181</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>167</v>
+        <v>119</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>120</v>
@@ -3506,7 +3699,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="25.5">
+    <row r="23" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>182</v>
       </c>
@@ -3520,7 +3713,7 @@
         <v>276</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>167</v>
+        <v>119</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>120</v>
@@ -3529,7 +3722,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="25.5">
+    <row r="24" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>183</v>
       </c>
@@ -3552,7 +3745,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="25.5">
+    <row r="25" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>185</v>
       </c>
@@ -3575,7 +3768,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>187</v>
       </c>
@@ -3598,7 +3791,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>192</v>
       </c>
@@ -3621,7 +3814,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="25.5">
+    <row r="28" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>194</v>
       </c>
@@ -3644,7 +3837,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="25.5">
+    <row r="29" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>197</v>
       </c>
@@ -3667,7 +3860,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="25.5">
+    <row r="30" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>199</v>
       </c>
@@ -3690,7 +3883,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="38.25">
+    <row r="31" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>201</v>
       </c>
@@ -3713,7 +3906,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="25.5">
+    <row r="32" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>204</v>
       </c>
@@ -3736,7 +3929,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="25.5">
+    <row r="33" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>207</v>
       </c>
@@ -3759,7 +3952,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>215</v>
       </c>
@@ -3782,7 +3975,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="25.5">
+    <row r="35" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>218</v>
       </c>
@@ -3805,7 +3998,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="25.5" hidden="1">
+    <row r="36" spans="1:10" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>221</v>
       </c>
@@ -3828,7 +4021,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="25.5" hidden="1">
+    <row r="37" spans="1:10" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>223</v>
       </c>
@@ -3851,7 +4044,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="25.5">
+    <row r="38" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>225</v>
       </c>
@@ -3865,7 +4058,7 @@
         <v>227</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>167</v>
+        <v>213</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>120</v>
@@ -3874,7 +4067,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>228</v>
       </c>
@@ -3888,7 +4081,7 @@
         <v>230</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>167</v>
+        <v>119</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>124</v>
@@ -3897,7 +4090,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="25.5">
+    <row r="40" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>231</v>
       </c>
@@ -3920,7 +4113,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="25.5">
+    <row r="41" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>234</v>
       </c>
@@ -3934,7 +4127,7 @@
         <v>235</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>167</v>
+        <v>119</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>120</v>
@@ -3943,7 +4136,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>236</v>
       </c>
@@ -3957,7 +4150,7 @@
         <v>237</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>167</v>
+        <v>119</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>120</v>
@@ -3966,7 +4159,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="25.5">
+    <row r="43" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>238</v>
       </c>
@@ -3989,7 +4182,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="25.5">
+    <row r="44" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>241</v>
       </c>
@@ -4003,7 +4196,7 @@
         <v>243</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>167</v>
+        <v>119</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>120</v>
@@ -4012,7 +4205,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="25.5">
+    <row r="45" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>242</v>
       </c>
@@ -4026,12 +4219,173 @@
         <v>245</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>167</v>
+        <v>213</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>120</v>
       </c>
       <c r="J45" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J52" s="1" t="s">
         <v>209</v>
       </c>
     </row>
@@ -4044,38 +4398,38 @@
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="F1:G1">
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="8" operator="equal">
       <formula>"Must"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1">
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
       <formula>"Could"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="7" operator="equal">
       <formula>"Should"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
       <formula>"Implement"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
       <formula>"Design"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
       <formula>"Must"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
       <formula>"Could"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
       <formula>"Should"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4091,19 +4445,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="3" customFormat="1" ht="51">
+    <row r="1" spans="1:20" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>85</v>
       </c>
@@ -4164,33 +4518,33 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="P1">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
       <formula>"Issue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>"Raised"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
       <formula>"Withdrawn"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4200,14 +4554,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" customWidth="1"/>
   </cols>

</xml_diff>